<commit_message>
Sigry correjido hoja de calculo
</commit_message>
<xml_diff>
--- a/doc/sigry/sigry2020.xlsx
+++ b/doc/sigry/sigry2020.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16799" uniqueCount="5073">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16800" uniqueCount="5073">
   <si>
     <t xml:space="preserve"> virtuemart_product_id</t>
   </si>
@@ -15452,8 +15452,8 @@
   </sheetPr>
   <dimension ref="A1:M1836"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A828" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B832" activeCellId="1" sqref="D454 B832"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -28853,12 +28853,15 @@
         <v>1303</v>
       </c>
     </row>
-    <row r="454" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="454" s="1" customFormat="true" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B454" s="1" t="s">
         <v>1211</v>
       </c>
       <c r="C454" s="2" t="s">
         <v>1304</v>
+      </c>
+      <c r="D454" s="2" t="s">
+        <v>1212</v>
       </c>
       <c r="E454" s="1" t="s">
         <v>1305</v>

</xml_diff>